<commit_message>
Add Assets to Config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spieler 1\Documents\UiPath\WeatherMailer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8437F124-4035-4050-B3A7-A2BB7B01A38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>APIKey</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
 </sst>
 </file>
@@ -223,7 +232,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -239,9 +248,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +288,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +394,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,11 +550,11 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.53125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="3" max="3" width="81.46484375" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -594,7 +603,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="42.75">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +613,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="28.5">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1623,11 +1632,11 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="3" max="3" width="75.46484375" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1665,7 +1674,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="28.5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="28.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1799,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="28.5">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2782,14 +2791,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="1" max="1" width="31.86328125" customWidth="1"/>
+    <col min="2" max="2" width="30.1328125" customWidth="1"/>
     <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="4" max="26" width="65.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2828,9 +2839,30 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Feat: add mock TransactionItem
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spieler 1\Documents\UiPath\WeatherMailer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8437F124-4035-4050-B3A7-A2BB7B01A38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F66AEE-DD10-45A4-9B43-2D24C879DC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -159,9 +156,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
     <t>APIKey</t>
   </si>
   <si>
@@ -169,6 +163,12 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>WeatherQueue</t>
+  </si>
+  <si>
+    <t>WeatherMailer</t>
   </si>
 </sst>
 </file>
@@ -221,10 +221,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
@@ -594,22 +594,22 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="42.75">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -618,10 +618,10 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1682,18 +1682,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="28.5">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1717,7 +1717,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1739,7 +1739,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1750,7 +1750,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1761,53 +1761,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.5">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2791,7 +2791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2811,7 +2811,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2841,26 +2841,26 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Feat: Add API Call
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spieler 1\Documents\UiPath\WeatherMailer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F66AEE-DD10-45A4-9B43-2D24C879DC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA194BF-DEB4-48CD-A681-3119F9A3918F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -162,13 +162,16 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>WeatherQueue</t>
   </si>
   <si>
     <t>WeatherMailer</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -597,7 +600,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -618,7 +621,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -2791,8 +2794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
@@ -2857,13 +2860,20 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>